<commit_message>
Included salinity intrusion length Tokar delta
</commit_message>
<xml_diff>
--- a/data/Reftable.xlsx
+++ b/data/Reftable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\engelen\OneDrive - Stichting Deltares\PhD\Synth_Delta\delta_aquifer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3184" documentId="10_ncr:100000_{2E746554-31FE-4657-A800-89661B694791}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{76F87A66-46F9-4A25-8F92-91071B738DAC}"/>
+  <xr:revisionPtr revIDLastSave="3187" documentId="10_ncr:100000_{2E746554-31FE-4657-A800-89661B694791}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{85768456-15DB-45E0-97C1-643BF0803E85}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27645" windowHeight="16440" activeTab="3" xr2:uid="{30BFF025-641A-48C0-8EBD-49846763B0B0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27645" windowHeight="16440" activeTab="2" xr2:uid="{30BFF025-641A-48C0-8EBD-49846763B0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry_Raw" sheetId="8" r:id="rId1"/>
@@ -4164,9 +4164,6 @@
     <t>(Noguiera et al., 2019)</t>
   </si>
   <si>
-    <t>No data in Nienhuis</t>
-  </si>
-  <si>
     <t>Inferred from location old beach ridges</t>
   </si>
   <si>
@@ -4213,6 +4210,9 @@
   </si>
   <si>
     <t>Values taken from NHI dataportal. Riverbed resistance taken from "Hoofdsysteem 2", since this layer represents the natural rivers. Recharge taken from the Veluwe area, as this is the main infiltration zone.</t>
+  </si>
+  <si>
+    <t>No data in Nienhuis, but Tidal factor very low other side of the Red Sea.</t>
   </si>
 </sst>
 </file>
@@ -6803,7 +6803,7 @@
         <v>230</v>
       </c>
       <c r="K5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7278,7 +7278,7 @@
         <v>0.3</v>
       </c>
       <c r="F22" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H22" t="s">
         <v>99</v>
@@ -7469,7 +7469,7 @@
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H29">
         <v>3</v>
@@ -7524,10 +7524,10 @@
         <v>0.5</v>
       </c>
       <c r="F31" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G31" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H31" t="s">
         <v>99</v>
@@ -7568,7 +7568,7 @@
         <v>153</v>
       </c>
       <c r="K32" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -7636,11 +7636,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25057E61-6EC8-4702-95F0-553682FCDA05}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7721,7 +7721,7 @@
         <v>386</v>
       </c>
       <c r="F3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -8229,7 +8229,7 @@
         <v>388</v>
       </c>
       <c r="F21" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -8255,16 +8255,19 @@
         <v>6000</v>
       </c>
       <c r="F22" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
-      <c r="H22" t="s">
-        <v>99</v>
+      <c r="H22">
+        <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>391</v>
+        <v>407</v>
+      </c>
+      <c r="J22" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -8613,8 +8616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E89A5B0-DBE8-48A0-8E4E-75422772F37C}">
   <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="E24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="O50" sqref="O50"/>
@@ -8758,10 +8761,10 @@
         <v>138</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>264</v>
@@ -11210,7 +11213,7 @@
         <v>151</v>
       </c>
       <c r="X34" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
@@ -11871,7 +11874,7 @@
         <v>99</v>
       </c>
       <c r="S43" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="T43" s="3" t="s">
         <v>99</v>
@@ -11883,7 +11886,7 @@
         <v>99</v>
       </c>
       <c r="W43" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
@@ -11942,7 +11945,7 @@
         <v>99</v>
       </c>
       <c r="S44" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="T44" s="3" t="s">
         <v>99</v>
@@ -11954,7 +11957,7 @@
         <v>99</v>
       </c>
       <c r="W44" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
@@ -12013,7 +12016,7 @@
         <v>99</v>
       </c>
       <c r="S45" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="T45" s="3" t="s">
         <v>99</v>
@@ -12025,7 +12028,7 @@
         <v>99</v>
       </c>
       <c r="W45" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
@@ -12084,7 +12087,7 @@
         <v>99</v>
       </c>
       <c r="S46" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="T46" s="3" t="s">
         <v>99</v>
@@ -12096,7 +12099,7 @@
         <v>99</v>
       </c>
       <c r="W46" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
@@ -12155,7 +12158,7 @@
         <v>99</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="T47" s="3" t="s">
         <v>99</v>
@@ -12167,7 +12170,7 @@
         <v>99</v>
       </c>
       <c r="W47" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
@@ -12240,10 +12243,10 @@
         <v>99</v>
       </c>
       <c r="W48" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="X48" s="3" t="s">
         <v>404</v>
-      </c>
-      <c r="X48" s="3" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
@@ -12314,10 +12317,10 @@
         <v>300</v>
       </c>
       <c r="W49" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="X49" t="s">
         <v>406</v>
-      </c>
-      <c r="X49" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>